<commit_message>
Updated marking data, gantt
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB86BD61-D8BE-4EAF-B2AA-6C2D2C82529B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9601A6-590D-4E84-A812-9A161BD352F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1088,7 +1088,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1122,7 @@
         <v>17</v>
       </c>
       <c r="H2" s="14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="34" t="s">
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="23">
         <v>0.85</v>
@@ -1492,7 +1492,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" s="8">
         <v>0.8</v>
@@ -1512,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" s="23">
         <v>0.85</v>
@@ -1592,10 +1592,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" s="8">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="13" spans="2:67" s="25" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added output, updated Gantt
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7347F64C-F4EC-4411-B18A-FB0A7A6EC8CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E3DC1-E0FC-4DDD-A2E0-77AB2D42E327}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1140,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="47" t="s">
@@ -1430,10 +1430,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="28">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
@@ -1492,10 +1492,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="23">
         <v>1</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:67" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1509,13 +1509,13 @@
         <v>4</v>
       </c>
       <c r="E8" s="27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="28">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1550,13 +1550,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="23">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>

</xml_diff>

<commit_message>
Updated data reader to process inline comments
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662B7C36-B236-4720-91B4-C4A3F2EAB970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5559CD-CB4C-4AD5-B93A-3097DFDF2322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1140,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="47" t="s">
@@ -1512,10 +1512,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G8" s="28">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1553,10 +1553,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9" s="23">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -1585,7 +1585,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="22">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D10" s="22">
         <v>2</v>
@@ -1606,7 +1606,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" s="22">
         <v>2</v>
@@ -1626,7 +1626,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="27">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D12" s="27">
         <v>5</v>
@@ -1667,7 +1667,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="22">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D13" s="22">
         <v>4</v>
@@ -1708,7 +1708,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="22">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D14" s="22">
         <v>2</v>

</xml_diff>

<commit_message>
Reworked repair cost printing
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF979D-4FF4-48D8-92B4-5ADC8C392DE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAE64DE-C580-4F81-A944-F96B91931C73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Project Planner</t>
   </si>
@@ -716,7 +716,120 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1106,7 +1219,7 @@
   <dimension ref="A1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1253,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="47" t="s">
@@ -1512,10 +1625,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="28">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1553,10 +1666,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" s="23">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -1579,31 +1692,51 @@
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
     </row>
-    <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+    <row r="10" spans="1:67" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="22">
         <v>2</v>
       </c>
       <c r="E10" s="22">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F10" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="23">
-        <v>0</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
     </row>
     <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C11" s="22">
         <v>8</v>
@@ -1621,97 +1754,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:67" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="22">
+        <v>8</v>
+      </c>
+      <c r="D12" s="22">
+        <v>2</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C13" s="27">
         <v>10</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D13" s="27">
         <v>5</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E13" s="27">
         <v>0</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F13" s="27">
         <v>0</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G13" s="28">
         <v>0</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="31"/>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="31"/>
-    </row>
-    <row r="13" spans="1:67" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21" t="s">
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
+    </row>
+    <row r="14" spans="1:67" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C14" s="22">
         <v>10</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D14" s="22">
         <v>4</v>
-      </c>
-      <c r="E13" s="22">
-        <v>0</v>
-      </c>
-      <c r="F13" s="22">
-        <v>0</v>
-      </c>
-      <c r="G13" s="23">
-        <v>0</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-    </row>
-    <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="22">
-        <v>13</v>
-      </c>
-      <c r="D14" s="22">
-        <v>2</v>
       </c>
       <c r="E14" s="22">
         <v>0</v>
@@ -1722,34 +1835,47 @@
       <c r="G14" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:67" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+    </row>
+    <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22">
+        <v>13</v>
+      </c>
+      <c r="D15" s="22">
+        <v>2</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0</v>
+      </c>
+      <c r="F15" s="22">
+        <v>0</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:67" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="33"/>
@@ -2214,40 +2340,66 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO31">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="H5:BO9 H11:BO31">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:BO32">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:BO10">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">

</xml_diff>

<commit_message>
Added collective CSV writer, added multi-write options
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAE64DE-C580-4F81-A944-F96B91931C73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8805548-414D-4D3B-BAD0-C93900782794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1253,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="47" t="s">
@@ -1625,10 +1625,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G8" s="28">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1707,10 +1707,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="23">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>

</xml_diff>